<commit_message>
balance changes in XLSX
</commit_message>
<xml_diff>
--- a/Assets/Data/shop_items.xlsx
+++ b/Assets/Data/shop_items.xlsx
@@ -1281,10 +1281,10 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,7 +1458,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="10">
-        <f t="shared" ref="H3:H33" si="0">IFERROR(E3/F3/S3,0)</f>
+        <f t="shared" ref="H3:H24" si="0">IFERROR(E3/F3/S3,0)</f>
         <v>3.3333333333333335</v>
       </c>
       <c r="I3" s="10">

</xml_diff>